<commit_message>
Excel agregado de columna codigo para preguntas y respuestas
</commit_message>
<xml_diff>
--- a/__mocks__/Preguntas Completas Por Tipo/preguntaObjetivasArriesgada.xlsx
+++ b/__mocks__/Preguntas Completas Por Tipo/preguntaObjetivasArriesgada.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sullc\Documents\TPI\Workspace\TPIntegrador\Angular\TPI-Front\src\assets\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tpi2\git\TPI-Front\__mocks__\Preguntas Completas Por Tipo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A566383E-3978-48C6-81A2-94AFA78D40FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990BDBF8-D4B1-4736-9382-07EDDF0BF77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{EA040AEE-35B0-4F5B-AEF3-29BB44B005B2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{EA040AEE-35B0-4F5B-AEF3-29BB44B005B2}"/>
   </bookViews>
   <sheets>
     <sheet name="categoria" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
   <si>
     <t>nombre</t>
   </si>
@@ -177,13 +177,88 @@
   </si>
   <si>
     <t>¿Qué es el análisis técnico en el contexto de la inversión y cómo puede ser útil para un inversor arriesgado?</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>PCA1</t>
+  </si>
+  <si>
+    <t>PCA2</t>
+  </si>
+  <si>
+    <t>PCA3</t>
+  </si>
+  <si>
+    <t>PCA4</t>
+  </si>
+  <si>
+    <t>PCA5</t>
+  </si>
+  <si>
+    <t>PCA6</t>
+  </si>
+  <si>
+    <t>RCA1</t>
+  </si>
+  <si>
+    <t>RCA2</t>
+  </si>
+  <si>
+    <t>RCA3</t>
+  </si>
+  <si>
+    <t>RCA4</t>
+  </si>
+  <si>
+    <t>RCA5</t>
+  </si>
+  <si>
+    <t>RCA6</t>
+  </si>
+  <si>
+    <t>RCA7</t>
+  </si>
+  <si>
+    <t>RCA8</t>
+  </si>
+  <si>
+    <t>RCA9</t>
+  </si>
+  <si>
+    <t>RCA10</t>
+  </si>
+  <si>
+    <t>RCA11</t>
+  </si>
+  <si>
+    <t>RCA12</t>
+  </si>
+  <si>
+    <t>RCA13</t>
+  </si>
+  <si>
+    <t>RCA14</t>
+  </si>
+  <si>
+    <t>RCA15</t>
+  </si>
+  <si>
+    <t>RCA16</t>
+  </si>
+  <si>
+    <t>RCA17</t>
+  </si>
+  <si>
+    <t>RCA18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,14 +268,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,19 +317,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,15 +649,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -602,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -627,12 +693,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -643,11 +709,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -662,19 +728,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E557A189-07BD-4DD4-AE4E-E2A608F405F0}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="194.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="194.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -693,8 +760,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -713,12 +783,15 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C3" t="s">
@@ -733,12 +806,15 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
@@ -753,8 +829,11 @@
       <c r="F4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -773,12 +852,15 @@
       <c r="F5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C6" t="s">
@@ -793,8 +875,11 @@
       <c r="F6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -813,7 +898,9 @@
       <c r="F7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -826,20 +913,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8759312-058C-4473-8FFB-A755D6FBD3C0}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="245.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="154.5703125" customWidth="1"/>
-    <col min="12" max="12" width="49.5703125" customWidth="1"/>
+    <col min="3" max="3" width="134.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -858,8 +945,11 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -876,12 +966,15 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -898,12 +991,15 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -920,12 +1016,15 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -942,12 +1041,15 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -964,12 +1066,15 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -986,12 +1091,15 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1008,12 +1116,15 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1030,12 +1141,15 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1052,12 +1166,15 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1074,12 +1191,15 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1096,12 +1216,15 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1118,12 +1241,15 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1140,12 +1266,15 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1162,11 +1291,14 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
-      </c>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1183,12 +1315,15 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1205,12 +1340,15 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1227,12 +1365,15 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1249,121 +1390,124 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I54" s="2"/>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I55" s="2"/>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I56" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="G19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1372,6 +1516,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100641454CD1F1E6E428D478A5DC37BACE7" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ef1708d85dca7377bd826ec35b62ca84">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xmlns:ns4="7798dcc9-908f-468f-826a-c598f412d6fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="69e720de7d55d3231f99e1910e4c19d8" ns3:_="" ns4:_="">
     <xsd:import namespace="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
@@ -1560,14 +1712,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1578,6 +1722,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46D3E674-3079-48B5-BFCB-0E49FE180026}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7798dcc9-908f-468f-826a-c598f412d6fc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7274836D-657B-48C7-97FD-AD88493854E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1596,23 +1757,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46D3E674-3079-48B5-BFCB-0E49FE180026}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7798dcc9-908f-468f-826a-c598f412d6fc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FE838D2-67DD-483F-BECE-425D67F53E63}">
   <ds:schemaRefs>

</xml_diff>